<commit_message>
new changes as form fail validation
</commit_message>
<xml_diff>
--- a/forms automation.xlsx
+++ b/forms automation.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20085" windowHeight="8700"/>
+    <workbookView windowWidth="20640" windowHeight="5175"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:I32"/>
+  <oleSize ref="A1:I31"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="70">
   <si>
     <t>No</t>
   </si>
@@ -41,6 +41,12 @@
     <t>https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/orthopaedics/disease/achilles-tendon-injury-symptoms-causes-treatment-recovery</t>
   </si>
   <si>
+    <t>✅ FORM SUBMITTED SUCCSESSFULLY!</t>
+  </si>
+  <si>
+    <t>Air Ambulance</t>
+  </si>
+  <si>
     <t>Become A Partner</t>
   </si>
   <si>
@@ -62,15 +68,15 @@
     <t>Contact us</t>
   </si>
   <si>
+    <t>Enquiry</t>
+  </si>
+  <si>
+    <t>https://www.medanta.org/contact-us</t>
+  </si>
+  <si>
     <t>Feedback</t>
   </si>
   <si>
-    <t>https://www.medanta.org/contact-us</t>
-  </si>
-  <si>
-    <t>Enquiry</t>
-  </si>
-  <si>
     <t>Others</t>
   </si>
   <si>
@@ -92,18 +98,15 @@
     <t>Elder care</t>
   </si>
   <si>
+    <t>Enquiry Form</t>
+  </si>
+  <si>
+    <t>https://www.medanta.org/elder-care-program</t>
+  </si>
+  <si>
     <t>Request a Callback</t>
   </si>
   <si>
-    <t>https://www.medanta.org/elder-care-program</t>
-  </si>
-  <si>
-    <t>Enroll now Form</t>
-  </si>
-  <si>
-    <t>Enquiry Form</t>
-  </si>
-  <si>
     <t>Header</t>
   </si>
   <si>
@@ -113,9 +116,21 @@
     <t>https://www.medanta.org/</t>
   </si>
   <si>
+    <t>HealthCheckup</t>
+  </si>
+  <si>
     <t>Homecare</t>
   </si>
   <si>
+    <t>Elder Care program</t>
+  </si>
+  <si>
+    <t>Elder Care program - https://www.medanta.org/home-care-service-program/elder-care-program</t>
+  </si>
+  <si>
+    <t>EnquiryNow</t>
+  </si>
+  <si>
     <t>https://www.medanta.org/home-care</t>
   </si>
   <si>
@@ -125,12 +140,6 @@
     <t>Stroke Rehabilitation Program - https://www.medanta.org/home-care-service-program/stroke-rehabilitation-program</t>
   </si>
   <si>
-    <t>Elder Care program</t>
-  </si>
-  <si>
-    <t>Elder Care program - https://www.medanta.org/home-care-service-program/elder-care-program</t>
-  </si>
-  <si>
     <t>International Patients</t>
   </si>
   <si>
@@ -170,39 +179,33 @@
     <t>https://www.medanta.org/plan-your-trip</t>
   </si>
   <si>
+    <t>Request an Estimate</t>
+  </si>
+  <si>
+    <t>Price Estimate form</t>
+  </si>
+  <si>
+    <t>https://www.medanta.org/international-patient/services/request-an-estimate</t>
+  </si>
+  <si>
+    <t>Second Opinion</t>
+  </si>
+  <si>
+    <t>https://www.medanta.org/second-opinion</t>
+  </si>
+  <si>
+    <t>Technology Detail Pages</t>
+  </si>
+  <si>
+    <t>https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/radiology/technology/ct-scan-on-wheels</t>
+  </si>
+  <si>
     <t>Telemedicine</t>
   </si>
   <si>
     <t>https://www.medanta.org/tele-medicine</t>
   </si>
   <si>
-    <t>Air Ambulance</t>
-  </si>
-  <si>
-    <t>HealthCheckup</t>
-  </si>
-  <si>
-    <t>Request an Estimate</t>
-  </si>
-  <si>
-    <t>Price Estimate form</t>
-  </si>
-  <si>
-    <t>https://www.medanta.org/international-patient/services/request-an-estimate</t>
-  </si>
-  <si>
-    <t>Second Opinion</t>
-  </si>
-  <si>
-    <t>https://www.medanta.org/second-opinion</t>
-  </si>
-  <si>
-    <t>Technology Detail Pages</t>
-  </si>
-  <si>
-    <t>https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/radiology/technology/ct-scan-on-wheels</t>
-  </si>
-  <si>
     <t>Treatment Detail</t>
   </si>
   <si>
@@ -218,7 +221,10 @@
     <t>https://www.medanta.org/eicu</t>
   </si>
   <si>
-    <t>PASS!</t>
+    <t>❌ FORM NOT SUBMITTED SUCCSESSFULLY! FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name=Test | Mobile=98210 | Email=wakemedantatest@gmail.com | Location=Gurugram | Errors =&gt; Mobile Error: Please enter 10 digit mobile number | </t>
   </si>
 </sst>
 </file>
@@ -226,10 +232,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -260,17 +266,131 @@
       <charset val="0"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
       <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
       <charset val="0"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -290,132 +410,18 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -444,91 +450,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,96 +624,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -656,6 +662,19 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -669,10 +688,10 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color auto="1"/>
-      </right>
-      <top/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -680,22 +699,11 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -714,9 +722,74 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -736,67 +809,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -814,152 +831,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -987,31 +1004,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1331,10 +1345,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E32"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1343,7 +1357,7 @@
     <col min="2" max="2" customWidth="true" style="3" width="25.1428571428571"/>
     <col min="3" max="3" customWidth="true" style="3" width="36.7142857142857"/>
     <col min="4" max="4" customWidth="true" style="3" width="138.0"/>
-    <col min="5" max="5" style="3" width="9.14285714285714"/>
+    <col min="5" max="5" customWidth="true" style="3" width="37.1428571428571"/>
     <col min="6" max="16384" style="1" width="9.14285714285714"/>
   </cols>
   <sheetData>
@@ -1378,7 +1392,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1390,16 +1404,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="10"/>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1411,16 +1421,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1431,95 +1441,97 @@
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:5">
+    <row r="6" s="2" customFormat="1" spans="1:9">
       <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:5">
       <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="E7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" s="2" customFormat="1" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:5">
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>19</v>
+      <c r="B8" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="9" s="2" customFormat="1" spans="1:9">
       <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1528,17 +1540,17 @@
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1549,14 +1561,18 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>24</v>
+      <c r="B11" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11"/>
+      <c r="D11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1566,14 +1582,16 @@
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>24</v>
+      <c r="B12" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="13"/>
-      <c r="E12"/>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1584,123 +1602,122 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="1:5">
+    <row r="14" s="2" customFormat="1" spans="1:9">
       <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>67</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:5">
       <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>33</v>
+      <c r="B15" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:5">
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="15" t="s">
+      <c r="B16" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>35</v>
+      <c r="C16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" spans="1:5">
       <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>37</v>
+      <c r="B17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" s="2" customFormat="1" spans="1:6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="1:5">
       <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="9" t="s">
+      <c r="B18" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>39</v>
       </c>
+      <c r="D18" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="E18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="19" s="2" customFormat="1" spans="1:6">
       <c r="A19" s="6">
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -1708,69 +1725,70 @@
       <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" s="1" customFormat="1" spans="1:5">
+    <row r="21" s="2" customFormat="1" spans="1:6">
       <c r="A21" s="6">
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>47</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="1:5">
       <c r="A22" s="6">
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" spans="1:5">
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>49</v>
+      <c r="B23" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E23" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="1" spans="1:5">
@@ -1778,16 +1796,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>52</v>
+        <v>14</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" spans="1:5">
@@ -1795,25 +1813,33 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="17"/>
+        <v>54</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="E25" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="1" spans="1:5">
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="17"/>
+      <c r="B26" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="E26" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" spans="1:5">
@@ -1821,33 +1847,33 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" spans="1:5">
       <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>58</v>
+      <c r="B28" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>59</v>
+        <v>29</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="E28" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="1" spans="1:5">
@@ -1855,16 +1881,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E29" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" spans="1:5">
@@ -1872,70 +1898,50 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E30" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" spans="1:5">
-      <c r="A31" s="6">
-        <v>30</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" s="1" customFormat="1" spans="1:5">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D10:D12"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/orthopaedics/disease/achilles-tendon-injury-symptoms-causes-treatment-recovery" tooltip="https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/orthopaedics/disease/achilles-tendon-injury-symptoms-causes-treatment-recovery"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://www.medanta.org/medanta-labs/become-a-partner" tooltip="https://www.medanta.org/medanta-labs/become-a-partner"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://www.medanta.org/patient-education-blog/omicron-variant-key-facts-you-need-to-know-in-2025" tooltip="https://www.medanta.org/patient-education-blog/omicron-variant-key-facts-you-need-to-know-in-2025"/>
-    <hyperlink ref="D21" r:id="rId4" display="https://www.medanta.org/medanta-pharmacy" tooltip="https://www.medanta.org/medanta-pharmacy"/>
+    <hyperlink ref="D4" r:id="rId2" display="https://www.medanta.org/medanta-labs/become-a-partner" tooltip="https://www.medanta.org/medanta-labs/become-a-partner"/>
+    <hyperlink ref="D5" r:id="rId3" display="https://www.medanta.org/patient-education-blog/omicron-variant-key-facts-you-need-to-know-in-2025" tooltip="https://www.medanta.org/patient-education-blog/omicron-variant-key-facts-you-need-to-know-in-2025"/>
     <hyperlink ref="D22" r:id="rId4" display="https://www.medanta.org/medanta-pharmacy" tooltip="https://www.medanta.org/medanta-pharmacy"/>
-    <hyperlink ref="D5" r:id="rId5" display="https://www.medanta.org/contact-us" tooltip="https://www.medanta.org/contact-us"/>
+    <hyperlink ref="D23" r:id="rId4" display="https://www.medanta.org/medanta-pharmacy" tooltip="https://www.medanta.org/medanta-pharmacy"/>
     <hyperlink ref="D6" r:id="rId5" display="https://www.medanta.org/contact-us" tooltip="https://www.medanta.org/contact-us"/>
     <hyperlink ref="D7" r:id="rId5" display="https://www.medanta.org/contact-us" tooltip="https://www.medanta.org/contact-us"/>
-    <hyperlink ref="D8" r:id="rId6" display="https://www.medanta.org/cpr" tooltip="https://www.medanta.org/cpr"/>
-    <hyperlink ref="D9" r:id="rId7" display="https://www.medanta.org/careers/events/cultural-events" tooltip="https://www.medanta.org/careers/events/cultural-events"/>
-    <hyperlink ref="D10" r:id="rId8" display="https://www.medanta.org/elder-care-program" tooltip="https://www.medanta.org/elder-care-program"/>
+    <hyperlink ref="D8" r:id="rId5" display="https://www.medanta.org/contact-us" tooltip="https://www.medanta.org/contact-us"/>
+    <hyperlink ref="D9" r:id="rId6" display="https://www.medanta.org/cpr" tooltip="https://www.medanta.org/cpr"/>
+    <hyperlink ref="D10" r:id="rId7" display="https://www.medanta.org/careers/events/cultural-events" tooltip="https://www.medanta.org/careers/events/cultural-events"/>
+    <hyperlink ref="D11" r:id="rId8" display="https://www.medanta.org/elder-care-program" tooltip="https://www.medanta.org/elder-care-program"/>
     <hyperlink ref="D13" r:id="rId9" display="https://www.medanta.org/" tooltip="https://www.medanta.org/"/>
-    <hyperlink ref="D14" r:id="rId10" display="https://www.medanta.org/home-care" tooltip="https://www.medanta.org/home-care"/>
-    <hyperlink ref="D15" r:id="rId10" display="https://www.medanta.org/home-care" tooltip="https://www.medanta.org/home-care"/>
-    <hyperlink ref="D18" r:id="rId11" display="https://www.medanta.org/international-patient" tooltip="https://www.medanta.org/international-patient"/>
-    <hyperlink ref="D19" r:id="rId12" display="https://www.medanta.org/ehc/hishealth-checkup/L1gz" tooltip="https://www.medanta.org/ehc/hishealth-checkup/L1gz"/>
-    <hyperlink ref="D20" r:id="rId13" display="https://www.medanta.org/medanta-labs" tooltip="https://www.medanta.org/medanta-labs"/>
-    <hyperlink ref="D23" r:id="rId14" display="https://www.medanta.org/plan-your-trip" tooltip="https://www.medanta.org/plan-your-trip"/>
-    <hyperlink ref="D27" r:id="rId15" display="https://www.medanta.org/international-patient/services/request-an-estimate" tooltip="https://www.medanta.org/international-patient/services/request-an-estimate"/>
-    <hyperlink ref="D28" r:id="rId16" display="https://www.medanta.org/second-opinion" tooltip="https://www.medanta.org/second-opinion"/>
-    <hyperlink ref="D29" r:id="rId17" display="https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/radiology/technology/ct-scan-on-wheels" tooltip="https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/radiology/technology/ct-scan-on-wheels"/>
-    <hyperlink ref="D30" r:id="rId18" display="https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/plastic-surgery/treatment/abdominoplasty-tummy-tuck-operation" tooltip="https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/plastic-surgery/treatment/abdominoplasty-tummy-tuck-operation"/>
-    <hyperlink ref="D31" r:id="rId19" display="https://www.medanta.org/eicu" tooltip="https://www.medanta.org/eicu"/>
+    <hyperlink ref="D17" r:id="rId10" display="https://www.medanta.org/home-care" tooltip="https://www.medanta.org/home-care"/>
+    <hyperlink ref="D16" r:id="rId10" display="https://www.medanta.org/home-care" tooltip="https://www.medanta.org/home-care"/>
+    <hyperlink ref="D19" r:id="rId11" display="https://www.medanta.org/international-patient" tooltip="https://www.medanta.org/international-patient"/>
+    <hyperlink ref="D20" r:id="rId12" display="https://www.medanta.org/ehc/hishealth-checkup/L1gz" tooltip="https://www.medanta.org/ehc/hishealth-checkup/L1gz"/>
+    <hyperlink ref="D21" r:id="rId13" display="https://www.medanta.org/medanta-labs" tooltip="https://www.medanta.org/medanta-labs"/>
+    <hyperlink ref="D24" r:id="rId14" display="https://www.medanta.org/plan-your-trip" tooltip="https://www.medanta.org/plan-your-trip"/>
+    <hyperlink ref="D25" r:id="rId15" display="https://www.medanta.org/international-patient/services/request-an-estimate" tooltip="https://www.medanta.org/international-patient/services/request-an-estimate"/>
+    <hyperlink ref="D26" r:id="rId16" display="https://www.medanta.org/second-opinion" tooltip="https://www.medanta.org/second-opinion"/>
+    <hyperlink ref="D27" r:id="rId17" display="https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/radiology/technology/ct-scan-on-wheels" tooltip="https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/radiology/technology/ct-scan-on-wheels"/>
+    <hyperlink ref="D29" r:id="rId18" display="https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/plastic-surgery/treatment/abdominoplasty-tummy-tuck-operation" tooltip="https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/plastic-surgery/treatment/abdominoplasty-tummy-tuck-operation"/>
+    <hyperlink ref="D30" r:id="rId19" display="https://www.medanta.org/eicu" tooltip="https://www.medanta.org/eicu"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
date added in excel
</commit_message>
<xml_diff>
--- a/forms automation.xlsx
+++ b/forms automation.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12375"/>
+    <workbookView windowWidth="19650" windowHeight="6135"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:I31"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
   <si>
     <t>No</t>
   </si>
@@ -40,6 +41,9 @@
     <t>https://www.medanta.org/hospitals-near-me/gurugram-hospital/speciality/orthopaedics/disease/achilles-tendon-injury-symptoms-causes-treatment-recovery</t>
   </si>
   <si>
+    <t>✅ FORM SUBMITTED SUCCESSFULLY!</t>
+  </si>
+  <si>
     <t>Air Ambulance</t>
   </si>
   <si>
@@ -217,7 +221,7 @@
     <t>https://www.medanta.org/eicu</t>
   </si>
   <si>
-    <t>✅ FORM SUBMITTED SUCCESSFULLY!</t>
+    <t>Date:</t>
   </si>
 </sst>
 </file>
@@ -225,10 +229,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -273,7 +277,75 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,19 +361,13 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -317,104 +383,42 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -443,43 +447,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,139 +603,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,6 +739,15 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -766,21 +779,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -796,11 +794,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -824,148 +828,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1338,20 +1342,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:L32"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="3" width="9.14285714285714"/>
-    <col min="2" max="2" customWidth="true" style="3" width="25.1428571428571"/>
-    <col min="3" max="3" customWidth="true" style="3" width="36.7142857142857"/>
-    <col min="4" max="4" customWidth="true" style="3" width="138.0"/>
-    <col min="5" max="5" customWidth="true" style="3" width="37.1428571428571"/>
-    <col min="6" max="16384" style="1" width="9.14285714285714"/>
+    <col min="1" max="1" width="9.14285714285714" style="3"/>
+    <col min="2" max="2" width="25.1428571428571" style="3" customWidth="1"/>
+    <col min="3" max="3" width="36.7142857142857" style="3" customWidth="1"/>
+    <col min="4" max="4" width="138" style="3" customWidth="1"/>
+    <col min="5" max="5" width="37.1428571428571" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15.75" spans="1:5">
@@ -1385,7 +1389,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1397,12 +1401,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="10"/>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1414,16 +1418,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1435,16 +1439,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1456,16 +1460,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1477,16 +1481,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:5">
@@ -1494,16 +1498,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" spans="1:9">
@@ -1511,16 +1515,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F9"/>
       <c r="G9" s="1"/>
@@ -1532,16 +1536,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1553,16 +1557,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1574,14 +1578,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1593,16 +1597,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1614,12 +1618,12 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1631,16 +1635,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:5">
@@ -1648,16 +1652,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" spans="1:5">
@@ -1665,16 +1669,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="1" spans="1:5">
@@ -1682,16 +1686,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1" spans="1:6">
@@ -1699,16 +1703,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -1717,16 +1721,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -1735,16 +1739,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -1753,16 +1757,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" spans="1:5">
@@ -1770,16 +1774,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="E23" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="1" spans="1:5">
@@ -1787,16 +1791,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" spans="1:5">
@@ -1804,16 +1808,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="1" spans="1:5">
@@ -1821,16 +1825,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E26" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="1" spans="1:5">
@@ -1838,16 +1842,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" spans="1:5">
@@ -1855,16 +1859,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E28" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="1" spans="1:5">
@@ -1872,16 +1876,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E29" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" spans="1:5">
@@ -1889,16 +1893,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E30" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" spans="1:5">
@@ -1907,6 +1911,11 @@
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>